<commit_message>
es werden mehrere Daten (KWs) aus der Excel-Datei geladen und die Buttons zur Auswahl der KW aktualiseren die Tabelle direkt mit
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Haushaltsbuch_2022.xlsx
+++ b/src/main/resources/excel/Haushaltsbuch_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larad\Dokumente\Programme\JetBrains\Projekte\HaushaltsbuchFX\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C616DC-3959-40ED-A150-53FD28AA9760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BD5AAA-92AC-401E-87D6-7B4E51E8487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26895" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{6242E93C-EC54-432C-80A4-85FF6AE47B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{6242E93C-EC54-432C-80A4-85FF6AE47B01}"/>
   </bookViews>
   <sheets>
     <sheet name="KW1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
   <si>
     <t>datum</t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>Einkaufen</t>
+  </si>
+  <si>
+    <t>Streaming</t>
+  </si>
+  <si>
+    <t>Sky Ticket</t>
+  </si>
+  <si>
+    <t>Rossmann</t>
+  </si>
+  <si>
+    <t>Drogerie</t>
+  </si>
+  <si>
+    <t>Flaschenpost</t>
+  </si>
+  <si>
+    <t>Gehalt</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Unterhosen</t>
+  </si>
+  <si>
+    <t>Kleidung</t>
+  </si>
+  <si>
+    <t>60° + 30° (d)</t>
   </si>
 </sst>
 </file>
@@ -442,14 +472,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCFF063-1330-4E9E-BF5C-18905E1153C5}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -477,7 +507,7 @@
         <v>44564</v>
       </c>
       <c r="B2" s="1">
-        <v>6.5</v>
+        <v>-6.5</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -494,7 +524,7 @@
         <v>44565</v>
       </c>
       <c r="B3" s="1">
-        <v>3.99</v>
+        <v>-3.99</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -511,7 +541,7 @@
         <v>44567</v>
       </c>
       <c r="B4" s="1">
-        <v>6.5</v>
+        <v>-6.5</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -528,7 +558,7 @@
         <v>44568</v>
       </c>
       <c r="B5" s="1">
-        <v>79.61</v>
+        <v>-79.61</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -586,18 +616,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8B1437-5F08-49C8-9115-AA5C75A99B48}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -618,6 +648,91 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44573</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-4.99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44575</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-80.34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44575</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-6.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44577</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-7.92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44577</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -625,18 +740,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0DAA48-9B2C-4EA7-87EC-85D07AE988D1}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -657,6 +772,40 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44582</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-74.47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44582</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-6.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -664,18 +813,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE192715-10BA-4811-B11B-CD212465E4FC}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -696,6 +845,88 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44586</v>
+      </c>
+      <c r="B2" s="1">
+        <v>230.24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44586</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-46.68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44587</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-45.98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44589</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-74.64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44589</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-6.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -705,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB979DC-A3C4-40EC-9DD4-548952A876BF}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
es können nur so viel KWs ausgewählt werden, wie tatsächlich im Haushaltbuch eingetragen sind
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Haushaltsbuch_2022.xlsx
+++ b/src/main/resources/excel/Haushaltsbuch_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larad\Dokumente\Programme\JetBrains\Projekte\HaushaltsbuchFX\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BD5AAA-92AC-401E-87D6-7B4E51E8487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381DB63A-AF30-4915-BE06-5E8324D30912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{6242E93C-EC54-432C-80A4-85FF6AE47B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{6242E93C-EC54-432C-80A4-85FF6AE47B01}"/>
   </bookViews>
   <sheets>
     <sheet name="KW1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="KW6" sheetId="6" r:id="rId6"/>
     <sheet name="KW7" sheetId="7" r:id="rId7"/>
     <sheet name="KW8" sheetId="8" r:id="rId8"/>
-    <sheet name="KW9" sheetId="9" r:id="rId9"/>
-    <sheet name="KW10" sheetId="10" r:id="rId10"/>
+    <sheet name="KW9" sheetId="11" r:id="rId9"/>
+    <sheet name="KW10" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="48">
   <si>
     <t>datum</t>
   </si>
@@ -114,6 +114,81 @@
   </si>
   <si>
     <t>60° + 30° (d)</t>
+  </si>
+  <si>
+    <t>30° (h)  + 60° (d)</t>
+  </si>
+  <si>
+    <t>Acer Nitro VG220</t>
+  </si>
+  <si>
+    <t>von Mama</t>
+  </si>
+  <si>
+    <t>Papa (Monitorhalterung)</t>
+  </si>
+  <si>
+    <t>Fabletics</t>
+  </si>
+  <si>
+    <t>Umbuchung</t>
+  </si>
+  <si>
+    <t>30° (d)</t>
+  </si>
+  <si>
+    <t>Bäcker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">von Robin </t>
+  </si>
+  <si>
+    <t>Film</t>
+  </si>
+  <si>
+    <t>Filme</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>Lisann Wii</t>
+  </si>
+  <si>
+    <t>Angelika</t>
+  </si>
+  <si>
+    <t>Snacks</t>
+  </si>
+  <si>
+    <t>von Robin</t>
+  </si>
+  <si>
+    <t>Amazon Prime</t>
+  </si>
+  <si>
+    <t>60° (d) + 30° (h)</t>
+  </si>
+  <si>
+    <t>Alex (Restaurant)</t>
+  </si>
+  <si>
+    <t>Essen gehen</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Mayersche</t>
+  </si>
+  <si>
+    <t>Bücher</t>
+  </si>
+  <si>
+    <t>Pille</t>
+  </si>
+  <si>
+    <t>Eis essen</t>
   </si>
 </sst>
 </file>
@@ -152,15 +227,259 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -473,7 +792,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,24 +890,40 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B5">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61F83B4-1150-4619-AA6C-2A2A2D97BDA1}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F44F1FA-1C9B-4AEA-A502-721BB6437043}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -609,7 +944,63 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>44629</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>44629</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-19.27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44629</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -619,7 +1010,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +1057,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>44575</v>
       </c>
       <c r="B3" s="1">
@@ -683,7 +1074,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>44575</v>
       </c>
       <c r="B4" s="1">
@@ -700,7 +1091,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>44577</v>
       </c>
       <c r="B5" s="1">
@@ -717,7 +1108,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>44577</v>
       </c>
       <c r="B6" s="1">
@@ -734,6 +1125,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -743,7 +1142,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +1172,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>44582</v>
       </c>
       <c r="B2" s="1">
@@ -790,7 +1189,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>44582</v>
       </c>
       <c r="B3" s="1">
@@ -807,6 +1206,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -816,7 +1223,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +1253,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>44586</v>
       </c>
       <c r="B2" s="1">
@@ -863,7 +1270,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>44586</v>
       </c>
       <c r="B3" s="1">
@@ -894,7 +1301,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>44589</v>
       </c>
       <c r="B5" s="1">
@@ -911,7 +1318,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>44589</v>
       </c>
       <c r="B6" s="1">
@@ -928,22 +1335,450 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB979DC-A3C4-40EC-9DD4-548952A876BF}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44594</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-133.38999999999999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44596</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-44.36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44597</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-6.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44597</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44597</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B90DA2-22ED-46FB-A205-28453F2CDA88}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>44600</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>44600</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-42.49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-49.95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B5" s="1">
+        <v>49.95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-67.650000000000006</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE3E607-4B5A-4094-82B7-9920CA5F73E9}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44608</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-11.75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>44610</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-8.11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44610</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44610</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-46.75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44611</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-6.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>44611</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-3.98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B7">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE4BEAF-7FEF-4093-AB6F-34A4B464AA11}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -966,25 +1801,174 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44614</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-16.18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44616</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44617</v>
+      </c>
+      <c r="B4" s="1">
+        <v>661.09</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44617</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-64.52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44618</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-67.900000000000006</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>44618</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44618</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-8.91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>44618</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-2.1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>44618</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B90DA2-22ED-46FB-A205-28453F2CDA88}">
-  <dimension ref="A1:E1"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0165A27-6BD3-465B-BA3F-BB34A4C28728}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1005,124 +1989,131 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44620</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44621</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-9.1999999999999993</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44623</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-95.94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44655</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-6.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44655</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-55.32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>44625</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44625</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-47.89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE3E607-4B5A-4094-82B7-9920CA5F73E9}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE4BEAF-7FEF-4093-AB6F-34A4B464AA11}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F5A0C7-475A-4B39-9DFB-81E1643734C8}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
neue Kategorien und HomePage Elemente hinzugefügt
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Haushaltsbuch_2022.xlsx
+++ b/src/main/resources/excel/Haushaltsbuch_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larad\Dokumente\Programme\JetBrains\Projekte\HaushaltsbuchFX\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381DB63A-AF30-4915-BE06-5E8324D30912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10166A3C-5466-4A5C-8DF9-42E56C89CE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{6242E93C-EC54-432C-80A4-85FF6AE47B01}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="9" xr2:uid="{6242E93C-EC54-432C-80A4-85FF6AE47B01}"/>
   </bookViews>
   <sheets>
     <sheet name="KW1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="49">
   <si>
     <t>datum</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Eis essen</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -261,6 +264,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -271,6 +284,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -281,6 +304,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -311,6 +344,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -321,6 +364,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -351,6 +404,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -401,81 +464,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -891,18 +894,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -915,7 +918,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,6 +990,9 @@
       </c>
       <c r="C4" t="s">
         <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
@@ -1126,10 +1132,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1207,10 +1213,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1223,7 +1229,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,6 +1285,9 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
@@ -1336,10 +1345,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1352,7 +1361,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,6 +1400,9 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
@@ -1465,10 +1477,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1481,7 +1493,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,6 +1532,9 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
@@ -1534,6 +1549,9 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
@@ -1565,6 +1583,9 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1602,10 +1623,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1618,7 +1639,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,6 +1712,9 @@
       <c r="C4" t="s">
         <v>31</v>
       </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
@@ -1756,10 +1780,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1772,7 +1796,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A10"/>
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,6 +1852,9 @@
       <c r="C3" t="s">
         <v>35</v>
       </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
@@ -1859,6 +1886,9 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
@@ -1924,6 +1954,9 @@
       <c r="C9" t="s">
         <v>37</v>
       </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
@@ -1938,16 +1971,19 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1960,7 +1996,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,6 +2069,9 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
@@ -2107,10 +2146,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>